<commit_message>
Chrono + bug sons
</commit_message>
<xml_diff>
--- a/Z_Organisation/TODOLIST.xlsx
+++ b/Z_Organisation/TODOLIST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brice\git\BFMM_SaveTheKoalas\Z_Organisation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HES\Semestre 4\RIA\Projet\BFMM_SaveTheKoalas\Z_Organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAA5CD5-C757-4068-AC8F-2BED6CE40618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B990C10-2186-46E8-9F16-03F1E3C12699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODOLIST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>TODOLIST</t>
   </si>
@@ -147,26 +147,13 @@
     <t>Geoloc</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Started - </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BUG</t>
-    </r>
-  </si>
-  <si>
     <t>BUGLIST</t>
   </si>
   <si>
     <t>Pas de DB, localstorage</t>
+  </si>
+  <si>
+    <t>Bug quand on meurt on peut pas restart</t>
   </si>
 </sst>
 </file>
@@ -296,14 +283,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,46 +680,46 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.54296875" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
     <col min="10" max="10" width="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.54296875" customWidth="1"/>
     <col min="15" max="15" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:15" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="I1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="I1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -776,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -812,7 +799,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -848,7 +835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -856,9 +843,9 @@
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="15">
+        <v>32</v>
+      </c>
+      <c r="D5" s="14">
         <v>43981</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -871,14 +858,16 @@
       <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="K5" s="4"/>
-      <c r="L5" s="15"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="7"/>
     </row>
-    <row r="6" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -890,7 +879,7 @@
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -903,10 +892,10 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="14"/>
+      <c r="N6" s="13"/>
       <c r="O6" s="7"/>
     </row>
-    <row r="7" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -932,7 +921,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -945,8 +934,8 @@
         <v>10</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="6" t="s">
-        <v>31</v>
+      <c r="G8" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="I8" s="2">
         <v>6</v>
@@ -958,7 +947,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -984,7 +973,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1010,7 +999,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1029,7 +1018,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1048,7 +1037,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Geoloc + hof bug
</commit_message>
<xml_diff>
--- a/Z_Organisation/TODOLIST.xlsx
+++ b/Z_Organisation/TODOLIST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HES\Semestre 4\RIA\Projet\BFMM_SaveTheKoalas\Z_Organisation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brice\git\BFMM_SaveTheKoalas\Z_Organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B990C10-2186-46E8-9F16-03F1E3C12699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBB30C1-23E2-4423-B410-FA722409E124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODOLIST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>TODOLIST</t>
   </si>
@@ -94,9 +94,6 @@
   <si>
     <t>Animation
 - Sprite</t>
-  </si>
-  <si>
-    <t>Phase d'incubation</t>
   </si>
   <si>
     <t>Niveaux
@@ -154,6 +151,15 @@
   </si>
   <si>
     <t>Bug quand on meurt on peut pas restart</t>
+  </si>
+  <si>
+    <t>Ecran well played (level successful)</t>
+  </si>
+  <si>
+    <t>STABLE</t>
+  </si>
+  <si>
+    <t>HallOfFame - level handling</t>
   </si>
 </sst>
 </file>
@@ -680,26 +686,26 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
     <col min="10" max="10" width="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.54296875" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.54296875" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.5703125" customWidth="1"/>
     <col min="15" max="15" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -710,7 +716,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="I1" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
@@ -719,7 +725,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -730,7 +736,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -751,7 +757,7 @@
         <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>12</v>
@@ -763,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -781,13 +787,13 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -795,16 +801,16 @@
         <v>14</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="O3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O3" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="12">
@@ -817,25 +823,25 @@
         <v>16</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2">
         <v>2</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -843,7 +849,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="14">
         <v>43981</v>
@@ -853,21 +859,25 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="2">
         <v>3</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -883,19 +893,25 @@
         <v>11</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="2">
         <v>4</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="N6" s="13"/>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O6" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -909,7 +925,7 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="2">
         <v>5</v>
@@ -921,7 +937,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -935,7 +951,7 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="2">
         <v>6</v>
@@ -947,12 +963,12 @@
       <c r="N8" s="4"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -960,8 +976,8 @@
         <v>14</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="5" t="s">
-        <v>19</v>
+      <c r="G9" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="I9" s="2">
         <v>7</v>
@@ -973,12 +989,12 @@
       <c r="N9" s="4"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -987,7 +1003,7 @@
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="2">
         <v>8</v>
@@ -999,15 +1015,22 @@
       <c r="N10" s="4"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" s="4"/>
+      <c r="G11" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I11" s="2">
         <v>9</v>
       </c>
@@ -1018,7 +1041,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1037,7 +1060,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Hof persistent bug resolved + draw avatar image in hof
</commit_message>
<xml_diff>
--- a/Z_Organisation/TODOLIST.xlsx
+++ b/Z_Organisation/TODOLIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brice\git\BFMM_SaveTheKoalas\Z_Organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBB30C1-23E2-4423-B410-FA722409E124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B5107E-5136-425D-A8B1-A7174BC01A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>TODOLIST</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>HallOfFame - level handling</t>
+  </si>
+  <si>
+    <t>HOF - Total bug game</t>
+  </si>
+  <si>
+    <t>Quand tu vas dans le hall of fame et que tu select un niveau et tu appuies sur la flèche du bas plantage total</t>
+  </si>
+  <si>
+    <t>Terminé (prevent default ligne 54 menu.js)</t>
   </si>
 </sst>
 </file>
@@ -686,7 +695,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +711,7 @@
     <col min="11" max="11" width="24.5703125" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
@@ -930,12 +939,22 @@
       <c r="I7" s="2">
         <v>5</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="J7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="14">
+        <v>43983</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="N7" s="4"/>
-      <c r="O7" s="6"/>
+      <c r="O7" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">

</xml_diff>

<commit_message>
Remove some images and update todolist
</commit_message>
<xml_diff>
--- a/Z_Organisation/TODOLIST.xlsx
+++ b/Z_Organisation/TODOLIST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brice\git\BFMM_SaveTheKoalas\Z_Organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B5107E-5136-425D-A8B1-A7174BC01A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C189E0-F626-47F5-B6CB-B366BFFEE37E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODOLIST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>TODOLIST</t>
   </si>
@@ -92,10 +92,6 @@
 - Temps et sauvegarde</t>
   </si>
   <si>
-    <t>Animation
-- Sprite</t>
-  </si>
-  <si>
     <t>Niveaux
 - Gestion des niveaux (1 fichier texte par niveau)
 - Gestion de l'artchitecture des niveaux</t>
@@ -108,9 +104,6 @@
   </si>
   <si>
     <t>En cours</t>
-  </si>
-  <si>
-    <t>Bug des maps (glitch)</t>
   </si>
   <si>
     <t>Success level indication (enter to restart)</t>
@@ -156,9 +149,6 @@
     <t>Ecran well played (level successful)</t>
   </si>
   <si>
-    <t>STABLE</t>
-  </si>
-  <si>
     <t>HallOfFame - level handling</t>
   </si>
   <si>
@@ -169,6 +159,37 @@
   </si>
   <si>
     <t>Terminé (prevent default ligne 54 menu.js)</t>
+  </si>
+  <si>
+    <t>Splash qui continue (sound)
+Victory/Game over sound en boucle</t>
+  </si>
+  <si>
+    <t>Bouton enter version mobile
+Autre détails version mobile</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>SAVE à la fin (SaveScore)</t>
+  </si>
+  <si>
+    <t>Brice + les srabs</t>
+  </si>
+  <si>
+    <t>Bug des maps (glitch)
+Bug des koalas</t>
+  </si>
+  <si>
+    <t>Persistent</t>
+  </si>
+  <si>
+    <t>Revoir et tester les niveaux</t>
+  </si>
+  <si>
+    <t>Rapport à fournir avec
+suggestion de patterns</t>
   </si>
 </sst>
 </file>
@@ -238,18 +259,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -264,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -285,16 +300,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -398,15 +403,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AFDB7351-89C5-4365-88F4-0834D3EB1367}" name="Tableau1" displayName="Tableau1" ref="A2:G13" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A2:G13" xr:uid="{536E52BB-1A47-462D-B67D-63881B891271}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AFDB7351-89C5-4365-88F4-0834D3EB1367}" name="Tableau1" displayName="Tableau1" ref="A2:G15" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A2:G15" xr:uid="{536E52BB-1A47-462D-B67D-63881B891271}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G13">
+    <sortCondition descending="1" ref="G2:G13"/>
+  </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{203DD695-71FD-499A-B0F0-50D9A24A0603}" name="ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{974A2E61-0EC1-4D93-9B96-4FF1DB779A6A}" name="Tâches" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{C934C37D-2008-4B4D-B19E-834E24F4EA39}" name="Commentaires" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{E9116AFA-D154-433C-A6FF-8E305BA9AFBE}" name="Visa" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{464E079D-29B5-4AE8-BCD1-1B125C5F0886}" name="Reponsable 1" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{FEBBDEA9-8EB6-4CCE-B4C5-D1E5B0EA1761}" name="Reponsable 2" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{203DD695-71FD-499A-B0F0-50D9A24A0603}" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{974A2E61-0EC1-4D93-9B96-4FF1DB779A6A}" name="Tâches" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{C934C37D-2008-4B4D-B19E-834E24F4EA39}" name="Commentaires" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E9116AFA-D154-433C-A6FF-8E305BA9AFBE}" name="Visa" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{464E079D-29B5-4AE8-BCD1-1B125C5F0886}" name="Reponsable 1" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{FEBBDEA9-8EB6-4CCE-B4C5-D1E5B0EA1761}" name="Reponsable 2" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{263CF17C-A9F9-4036-8509-DC68EB5EF28D}" name="Etat"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -414,15 +422,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EE173EC5-9A7D-444B-BBD8-997083982114}" name="Tableau13" displayName="Tableau13" ref="I2:O12" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EE173EC5-9A7D-444B-BBD8-997083982114}" name="Tableau13" displayName="Tableau13" ref="I2:O12" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="I2:O12" xr:uid="{CF91EDB4-2461-41B1-9EC3-2FBEA55D0FCA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:O12">
+    <sortCondition ref="O2:O12"/>
+  </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B3AC7E44-3A15-456C-BA95-2911A63FFABC}" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{8C2AE51A-9736-4DB4-9C1A-E9CDF16D332D}" name="Tâches" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B63A9336-B24D-4D77-8F0C-28EAC4D835DA}" name="Commentaires" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{5231D9EA-F18B-4678-844A-21DB12A59DBE}" name="Visa" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{7757919C-875E-422A-9107-646E2386E1C8}" name="Reponsable 1" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{A7F19E45-B56D-4E73-B369-40703E103464}" name="Reponsable 2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B3AC7E44-3A15-456C-BA95-2911A63FFABC}" name="ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{8C2AE51A-9736-4DB4-9C1A-E9CDF16D332D}" name="Tâches" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{B63A9336-B24D-4D77-8F0C-28EAC4D835DA}" name="Commentaires" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{5231D9EA-F18B-4678-844A-21DB12A59DBE}" name="Visa" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{7757919C-875E-422A-9107-646E2386E1C8}" name="Reponsable 1" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{A7F19E45-B56D-4E73-B369-40703E103464}" name="Reponsable 2" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{BAF49D19-34CB-4534-B093-DAE1ED04455A}" name="Etat"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -692,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +715,8 @@
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
     <col min="10" max="10" width="43" bestFit="1" customWidth="1"/>
@@ -715,24 +727,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="I1" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="I1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -745,7 +757,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -766,7 +778,7 @@
         <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>12</v>
@@ -786,7 +798,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="12">
+      <c r="D3" s="8">
         <v>43977</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -796,22 +808,24 @@
         <v>14</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="O3" s="6" t="s">
-        <v>34</v>
+      <c r="O3" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -819,10 +833,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="12">
+      <c r="D4" s="8">
         <v>43977</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -832,162 +846,164 @@
         <v>16</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="14">
-        <v>43981</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="4"/>
       <c r="G5" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K5" s="4"/>
-      <c r="L5" s="14"/>
+      <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="13"/>
+        <v>14</v>
+      </c>
+      <c r="N6" s="4"/>
       <c r="O6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="6" t="s">
-        <v>22</v>
+      <c r="G7" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="I7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="14">
-        <v>43983</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
       <c r="M7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="9"/>
       <c r="O7" s="7" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="2">
-        <v>6</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="10">
+        <v>43983</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="6"/>
+      <c r="O8" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -995,8 +1011,8 @@
         <v>14</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="6" t="s">
-        <v>22</v>
+      <c r="G9" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="I9" s="2">
         <v>7</v>
@@ -1010,19 +1026,23 @@
     </row>
     <row r="10" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="10">
+        <v>43981</v>
+      </c>
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="6" t="s">
-        <v>22</v>
+      <c r="G10" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="I10" s="2">
         <v>8</v>
@@ -1036,19 +1056,19 @@
     </row>
     <row r="11" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="7" t="s">
-        <v>20</v>
+      <c r="G11" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="I11" s="2">
         <v>9</v>
@@ -1064,11 +1084,18 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="F12" s="4"/>
+      <c r="G12" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="I12" s="2">
         <v>10</v>
       </c>
@@ -1080,19 +1107,67 @@
       <c r="O12" s="6"/>
     </row>
     <row r="13" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>